<commit_message>
DataGenFromFile is going on ...
</commit_message>
<xml_diff>
--- a/Data/gen_data/config.xlsx
+++ b/Data/gen_data/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rezakarbasi/PersonalFiles/Projects/1_DarCProj/MSE Project/Simulator App/EEW_simulator/Data/gen_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF4839C-5FF9-084A-8B70-72D9A15C5F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC228B53-CCC0-1A44-B535-23188908EF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="26740" windowHeight="15680" xr2:uid="{0326DF07-B248-C84E-A909-013977109545}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="26740" windowHeight="15680" activeTab="7" xr2:uid="{0326DF07-B248-C84E-A909-013977109545}"/>
   </bookViews>
   <sheets>
     <sheet name="C1-HORIZONTAL" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="stations" sheetId="12" r:id="rId7"/>
     <sheet name="earthquake" sheetId="13" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
   <si>
     <t>longitude</t>
   </si>
@@ -87,6 +87,12 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>sigma</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -471,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF746F26-E354-B043-88B0-FBDD98A18040}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -553,35 +559,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1459028402374916</v>
+        <v>4.150831505670884</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1552045436922773</v>
+        <v>4.1494092633389306</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1350447781289077</v>
+        <v>4.162534543678432</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.159005381034687</v>
+        <v>4.1308392419306044</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1660558833023709</v>
+        <v>4.1328466926949634</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1703840228376032</v>
+        <v>4.1285197917952301</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6350349735814111</v>
+        <v>3.6593804175810956</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6648897135591509</v>
+        <v>3.6447191569070481</v>
       </c>
       <c r="M3" s="1">
         <v>4.1500000000000004</v>
@@ -597,35 +603,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1312315453418655</v>
+        <v>4.1601644580581283</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1251732525259408</v>
+        <v>4.1448033254006651</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1375289646808433</v>
+        <v>4.1433913958284778</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1364606851937085</v>
+        <v>4.1559996621027633</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1748525509200984</v>
+        <v>4.1319312441668297</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1728111788305062</v>
+        <v>4.1439485117514057</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6738080673729607</v>
+        <v>3.6506919034552165</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6609369737134703</v>
+        <v>3.6378740526900191</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -637,35 +643,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1529459504386557</v>
+        <v>4.1317963142235552</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1329026176718235</v>
+        <v>4.1422839276076004</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1616031010306891</v>
+        <v>4.158985698512522</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1478859012318345</v>
+        <v>4.1335027666603787</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1573666282889077</v>
+        <v>4.1571099687542041</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1261952697420039</v>
+        <v>4.1535182896406111</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6302807633653993</v>
+        <v>3.6345872045747445</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6687976968767142</v>
+        <v>3.6467418719848479</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -675,35 +681,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1640411069550698</v>
+        <v>4.1642482868619624</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1327471602568595</v>
+        <v>4.1422813717646774</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1322060349037457</v>
+        <v>4.1489958323807175</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1483198722085053</v>
+        <v>4.1410787220625318</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1635777923827133</v>
+        <v>4.1312492137283092</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1371918375865882</v>
+        <v>4.128840066191354</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6559615751331722</v>
+        <v>3.6557377631838266</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6460103026098576</v>
+        <v>3.6298774989578404</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -803,35 +809,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62310238555461595</v>
+        <v>0.62462052867515072</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62187783352385639</v>
+        <v>0.62177451687773433</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62461949806745298</v>
+        <v>0.62215819302109754</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62097783893009206</v>
+        <v>0.6209098253130827</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6206568567600671</v>
+        <v>0.62528025225175721</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62085329631915664</v>
+        <v>0.62525540844523608</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67734605160002781</v>
+        <v>0.68040078110551316</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67674475240961951</v>
+        <v>0.67666528508861423</v>
       </c>
       <c r="M3" s="1">
         <v>0.623</v>
@@ -847,35 +853,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62073377574999022</v>
+        <v>0.62101678129511939</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62225989112445756</v>
+        <v>0.62183827504097322</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62496452701513527</v>
+        <v>0.62474844284562414</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62415960342828736</v>
+        <v>0.62076449420118751</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62446427747970013</v>
+        <v>0.62469748902211375</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62506579904523896</v>
+        <v>0.62455625805688597</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67888717504431306</v>
+        <v>0.68033604001576897</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.6766775619436568</v>
+        <v>0.68021790427578221</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -887,35 +893,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62514443422508703</v>
+        <v>0.6252226461083219</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62438128517847202</v>
+        <v>0.6214830922531861</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62141397682671551</v>
+        <v>0.62378400307142245</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62215719512444589</v>
+        <v>0.62307804627391272</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62106208033034171</v>
+        <v>0.62542120784993294</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62130747517812679</v>
+        <v>0.62392930559930948</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67931933581484638</v>
+        <v>0.67974397117640095</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67566904395079763</v>
+        <v>0.6768926906639724</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -925,35 +931,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6219065420044001</v>
+        <v>0.62124809838772466</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62115218801402461</v>
+        <v>0.62192156482555028</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62482419154972468</v>
+        <v>0.62206733769531175</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62341261851995156</v>
+        <v>0.62327374413504777</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62255483209428264</v>
+        <v>0.62255968168106379</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62464813996435786</v>
+        <v>0.62072317370371788</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67950573450448659</v>
+        <v>0.6767839795519458</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67667161889690741</v>
+        <v>0.68004660757300062</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1053,35 +1059,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96035354708729159</v>
+        <v>-0.9604809875312067</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96247435115731583</v>
+        <v>-0.96073095222191318</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95921916527086482</v>
+        <v>-0.96158333623836945</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95881154770175903</v>
+        <v>-0.95836203831013411</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95785047905315979</v>
+        <v>-0.95792455550664934</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96011794140580864</v>
+        <v>-0.95778244163333204</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.95061614455026389</v>
+        <v>-0.94961336759143811</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.95178817967214713</v>
+        <v>-0.95119999391127974</v>
       </c>
       <c r="M3" s="1">
         <v>-0.96</v>
@@ -1097,35 +1103,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.9619719711885717</v>
+        <v>-0.96121730019437246</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96160651197195068</v>
+        <v>-0.96043695687006825</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96070283851044236</v>
+        <v>-0.95946400017086664</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96067529713123567</v>
+        <v>-0.96204960969069553</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95899501028463485</v>
+        <v>-0.95854824298813179</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96124380840098123</v>
+        <v>-0.96026737106563276</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.94920718965796103</v>
+        <v>-0.95044661270687392</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.95106066298465985</v>
+        <v>-0.94769553612628188</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1137,35 +1143,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96099275302624765</v>
+        <v>-0.96224372900143751</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96228628759224033</v>
+        <v>-0.9599886698295742</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96146400474086913</v>
+        <v>-0.95964316206867495</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96165610012733393</v>
+        <v>-0.96047670396341855</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96085607091609992</v>
+        <v>-0.95866565412549221</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96159307757637569</v>
+        <v>-0.96147386303708049</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.94867187126942731</v>
+        <v>-0.95015492001573221</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.94795761039557636</v>
+        <v>-0.94788254708453112</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1175,35 +1181,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.9589858793341115</v>
+        <v>-0.96159594005963434</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96177352421639772</v>
+        <v>-0.95922190098422155</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96234536255881675</v>
+        <v>-0.9599513372106363</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96103392997569692</v>
+        <v>-0.95839747398191344</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96131754470633057</v>
+        <v>-0.95921095174567816</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96060158340708601</v>
+        <v>-0.95831608556733261</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.94867234070219664</v>
+        <v>-0.95100926465514657</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.95020326531733623</v>
+        <v>-0.94831427503390664</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1303,35 +1309,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.450083860063792</v>
+        <v>3.4423402614829013</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4553113364034664</v>
+        <v>3.4431428465673468</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4793061818702364</v>
+        <v>3.4827709103752009</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4652820077085362</v>
+        <v>3.4580866608115475</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4658385158355092</v>
+        <v>3.4740769792691979</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4519300612968586</v>
+        <v>3.446009033339978</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0121434825467679</v>
+        <v>3.0398758466333367</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0505332749460221</v>
+        <v>3.0241869476215903</v>
       </c>
       <c r="M3">
         <v>3.46</v>
@@ -1347,35 +1353,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4829917865380655</v>
+        <v>3.4747480536775894</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4547025938446709</v>
+        <v>3.4641418695302972</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4586865284239585</v>
+        <v>3.479532136242542</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4416701542539614</v>
+        <v>3.4446161861668378</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4605213142011908</v>
+        <v>3.4400636522922254</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4825914713727215</v>
+        <v>3.4488915719994906</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0439178353951073</v>
+        <v>3.0491247136349493</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0103249164917019</v>
+        <v>3.0405273314180832</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1387,35 +1393,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4552807026076624</v>
+        <v>3.4586910429354423</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4653533000087204</v>
+        <v>3.4690468450924712</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4810533406491149</v>
+        <v>3.4704110858309014</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4680921591250886</v>
+        <v>3.4606730499810396</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4470855873947324</v>
+        <v>3.4819768288880333</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4616124467295801</v>
+        <v>3.4394522883020335</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0070386626690229</v>
+        <v>3.0487257749458498</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.023024708586338</v>
+        <v>3.0288681209114716</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1425,35 +1431,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4811349835155196</v>
+        <v>3.4617097214018679</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4739299959650478</v>
+        <v>3.4455374716597253</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4498143573521443</v>
+        <v>3.4729532961972227</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4375372117232561</v>
+        <v>3.4618853819090956</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4717644185091028</v>
+        <v>3.4661253166236485</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4702867131376709</v>
+        <v>3.4759480939281566</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0200929757739017</v>
+        <v>3.0336038708225717</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0265290184728872</v>
+        <v>3.0192443834801299</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1553,35 +1559,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63159540414927762</v>
+        <v>0.63609146518755499</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63410145481667279</v>
+        <v>0.63758412198805647</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.636171412617348</v>
+        <v>0.63630796703882953</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63054656737267045</v>
+        <v>0.63273395966991719</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6370203836922933</v>
+        <v>0.63833463732076168</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6362680555923601</v>
+        <v>0.63391913421946322</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73625401961923742</v>
+        <v>0.72829028171835086</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.72926891648457237</v>
+        <v>0.73017123178132404</v>
       </c>
       <c r="M3">
         <v>0.63500000000000001</v>
@@ -1597,35 +1603,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6323194371413916</v>
+        <v>0.63012981695691117</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63935516934009917</v>
+        <v>0.63981758356775542</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63818268937110811</v>
+        <v>0.63776054983007213</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63352716198424863</v>
+        <v>0.63590452552670917</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63157691202495425</v>
+        <v>0.63047333235354064</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63819142853418664</v>
+        <v>0.63709195590171297</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73494938703782853</v>
+        <v>0.73454105403509828</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73545986007483166</v>
+        <v>0.73601755611126851</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1637,35 +1643,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63451903194718418</v>
+        <v>0.63575222037503065</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63130987093312607</v>
+        <v>0.631943327051673</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6344515808433373</v>
+        <v>0.63427262075820534</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63446174132064359</v>
+        <v>0.63079959955608167</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63780002911054101</v>
+        <v>0.63857552465018808</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63367932137992145</v>
+        <v>0.63971488366814844</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.72716190439649142</v>
+        <v>0.72772077475680852</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73202421040238463</v>
+        <v>0.72810033932824181</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1675,35 +1681,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6334372018679566</v>
+        <v>0.63232374344214426</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63914372927816043</v>
+        <v>0.63223687646479865</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63593587291666309</v>
+        <v>0.63601691045370856</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63927921631424511</v>
+        <v>0.63737645290236167</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63238463520434041</v>
+        <v>0.63319052529220587</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63310409264961476</v>
+        <v>0.630669159421962</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73223696113231596</v>
+        <v>0.73347533002787979</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73413295560674829</v>
+        <v>0.73565199753835286</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1803,35 +1809,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99523867720107717</v>
+        <v>-0.995601695194824</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99682783050535784</v>
+        <v>-0.9960560723407339</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99657945045648921</v>
+        <v>-0.99603865207433895</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99549380518729957</v>
+        <v>-0.99697726476565818</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99612709665012777</v>
+        <v>-0.99584359921900267</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99568038400292247</v>
+        <v>-0.99601080518648799</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0302533576541661</v>
+        <v>-1.0307581444394354</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0303697244537258</v>
+        <v>-1.0293654166020889</v>
       </c>
       <c r="M3">
         <v>-0.996</v>
@@ -1847,35 +1853,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99554471762045427</v>
+        <v>-0.99617407204149799</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99541538772019922</v>
+        <v>-0.99570309333458884</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99644040166012116</v>
+        <v>-0.99606251214972608</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99601004872764698</v>
+        <v>-0.99630677226578157</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99524067210227796</v>
+        <v>-0.99618687623307611</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99663069421699191</v>
+        <v>-0.99653080926953264</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0299840629595836</v>
+        <v>-1.0298993723680303</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0302698954611669</v>
+        <v>-1.0300855198680205</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1887,35 +1893,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99652361454146599</v>
+        <v>-0.99620257271636048</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99512833339585183</v>
+        <v>-0.9965126957353394</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99670033526864499</v>
+        <v>-0.99664294209399018</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99697042058310581</v>
+        <v>-0.99514930834559212</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99688411883819139</v>
+        <v>-0.99626402644359191</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99662991086674868</v>
+        <v>-0.99570205869861406</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0304779207171908</v>
+        <v>-1.0295583326609379</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0307205908245833</v>
+        <v>-1.0301411347335236</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1925,35 +1931,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99564765847090786</v>
+        <v>-0.99634415656670894</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99568021919049388</v>
+        <v>-0.99639295598337563</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.9954765994072603</v>
+        <v>-0.99625238802238092</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99617229567639831</v>
+        <v>-0.99618328045874449</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99621947188808413</v>
+        <v>-0.99655091789074035</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99697919823063497</v>
+        <v>-0.99663308239284742</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0305635343664414</v>
+        <v>-1.0296719655518209</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0308217146038272</v>
+        <v>-1.0293032948419134</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1988,101 +1994,101 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <f ca="1">35.6+0.4*RAND()</f>
-        <v>35.905010696368606</v>
+        <v>35.660897155904465</v>
       </c>
       <c r="B2">
         <f ca="1">51.7+RAND()</f>
-        <v>52.177260526143314</v>
+        <v>52.030785608078865</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ref="A3:A11" ca="1" si="0">35.6+0.4*RAND()</f>
-        <v>35.711422138938751</v>
+        <v>35.858119579593307</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B11" ca="1" si="1">51.7+RAND()</f>
-        <v>52.039081949645606</v>
+        <v>52.532408336111693</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>35.927132962954985</v>
+        <v>35.77477564777174</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>52.360553527075062</v>
+        <v>52.477476756511237</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>35.777768240519173</v>
+        <v>35.691683183207246</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>52.611480430610193</v>
+        <v>52.658458248985184</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>35.862288222313559</v>
+        <v>35.785006804764151</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>52.418102493305803</v>
+        <v>52.141011659607301</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>35.602337311546123</v>
+        <v>35.933004558204289</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>51.836927934874154</v>
+        <v>51.908052531462651</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>35.761916149965543</v>
+        <v>35.946562789776124</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>52.590933853854601</v>
+        <v>52.420783100760005</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>35.746320667197786</v>
+        <v>35.88677743821993</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>52.122231471929169</v>
+        <v>52.446211222639583</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>35.767285172125817</v>
+        <v>35.637596983505716</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>51.748040764692817</v>
+        <v>52.281854425182829</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>35.632014199983203</v>
+        <v>35.805762791872461</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>52.455674692282919</v>
+        <v>52.218614446311442</v>
       </c>
     </row>
   </sheetData>
@@ -2092,15 +2098,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E20358-110C-584C-AD76-D34B5149820A}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2114,13 +2120,16 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>35.735599999999998</v>
       </c>
@@ -2140,6 +2149,9 @@
       </c>
       <c r="F2">
         <v>5.2</v>
+      </c>
+      <c r="G2">
+        <v>0.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
max stations added to the project + random seed removed from data generators
</commit_message>
<xml_diff>
--- a/Data/gen_data/config.xlsx
+++ b/Data/gen_data/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rezakarbasi/PersonalFiles/Projects/1_DarCProj/MSE Project/Simulator App/EEW_simulator/Data/gen_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E6917A-B25B-B149-BA86-95568F1461C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3405ED46-4943-2E42-B99B-D3EBC9BEEB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="26740" windowHeight="15680" activeTab="7" xr2:uid="{0326DF07-B248-C84E-A909-013977109545}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="26740" windowHeight="15680" activeTab="6" xr2:uid="{0326DF07-B248-C84E-A909-013977109545}"/>
   </bookViews>
   <sheets>
     <sheet name="C1-HORIZONTAL" sheetId="1" r:id="rId1"/>
@@ -562,35 +562,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1522196090951971</v>
+        <v>4.1324275364989589</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1324998781565849</v>
+        <v>4.1341065032872368</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1479102688435248</v>
+        <v>4.1576830709491732</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1642328891365512</v>
+        <v>4.1488490617591864</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1430938747017834</v>
+        <v>4.1474930244022321</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1469999255946961</v>
+        <v>4.1548560735468065</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6542425559159009</v>
+        <v>3.6539965919083888</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6288387227223899</v>
+        <v>3.6320470417474309</v>
       </c>
       <c r="M3" s="1">
         <v>4.1500000000000004</v>
@@ -606,35 +606,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1273770203138991</v>
+        <v>4.1403576330015861</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1574290833228797</v>
+        <v>4.1272805594149293</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1614661846996581</v>
+        <v>4.1306416054546098</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1618205187359907</v>
+        <v>4.1704647899462355</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1518757708852894</v>
+        <v>4.1283513261014866</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1728149728531845</v>
+        <v>4.1439443911997023</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6338354905554833</v>
+        <v>3.6310478905394059</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6704977951513555</v>
+        <v>3.6465240596048898</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -646,35 +646,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1538460752585333</v>
+        <v>4.155930185162954</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.139298730304672</v>
+        <v>4.1411701380411028</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1364159672971672</v>
+        <v>4.1375357749445669</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1251192620742732</v>
+        <v>4.1418990605580488</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1364410717944597</v>
+        <v>4.1740969288075682</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1524121529474209</v>
+        <v>4.1734578793561274</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.651929795697324</v>
+        <v>3.6453817717163295</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6594812040405018</v>
+        <v>3.6420538537551099</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -684,35 +684,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1506955851762131</v>
+        <v>4.1694380174133281</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.154559903723495</v>
+        <v>4.1597079424078913</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1682667719449915</v>
+        <v>4.1695264956926428</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1554193289678825</v>
+        <v>4.1490666597696677</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1486822245041548</v>
+        <v>4.1432297611038011</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>4.1558308360623091</v>
+        <v>4.1293420308694717</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6521094883129361</v>
+        <v>3.6621287990825526</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.6429704558314757</v>
+        <v>3.6727999318347657</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -812,35 +812,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62528552658281678</v>
+        <v>0.62071634153430855</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62136073887784771</v>
+        <v>0.62315921036275856</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62364435110309036</v>
+        <v>0.62146738479721875</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62405566126571033</v>
+        <v>0.62206762170921148</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6237847365939494</v>
+        <v>0.62429047986730102</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62504020515616077</v>
+        <v>0.62250646259605746</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.68033921881270965</v>
+        <v>0.67828909462668396</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67813461513606488</v>
+        <v>0.67798741530418261</v>
       </c>
       <c r="M3" s="1">
         <v>0.623</v>
@@ -856,35 +856,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62195606548054161</v>
+        <v>0.62286263647108986</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6240451800089547</v>
+        <v>0.62390876413087326</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62509959092896628</v>
+        <v>0.621064649908595</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62522666842157681</v>
+        <v>0.62317565654679041</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62389621102437576</v>
+        <v>0.62503553783992483</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62257497338283374</v>
+        <v>0.62291063889479581</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67927486119701208</v>
+        <v>0.68047838130543037</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67959119691291847</v>
+        <v>0.67857961370871611</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -896,35 +896,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62529244049329602</v>
+        <v>0.62328918598423089</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62100061500001758</v>
+        <v>0.62154536493167567</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62266945580757926</v>
+        <v>0.62415366624392665</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62221379659572007</v>
+        <v>0.6245474468119635</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62353756960826345</v>
+        <v>0.62078620873969625</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62193160159537531</v>
+        <v>0.62471195476368124</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67977745804597456</v>
+        <v>0.67874206375638579</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67702055324674726</v>
+        <v>0.67736923404954352</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -934,35 +934,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62366168518568665</v>
+        <v>0.62129624812658302</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62359936565663621</v>
+        <v>0.62146640732525749</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6226834991764717</v>
+        <v>0.62370667759400222</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62242643433889611</v>
+        <v>0.62420232088533356</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.62340800238303418</v>
+        <v>0.62346668219018297</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6249179505900162</v>
+        <v>0.62056947488595393</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.6795657767263058</v>
+        <v>0.67904754634583619</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.67899443473715859</v>
+        <v>0.6760129009613125</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1062,35 +1062,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95977143274214327</v>
+        <v>-0.95941371008648013</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95895798308888625</v>
+        <v>-0.96073000035415668</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96083823299741966</v>
+        <v>-0.96147616695271121</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95882481725665591</v>
+        <v>-0.95930013807713144</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96080569688989348</v>
+        <v>-0.96168895438267987</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95900520451883775</v>
+        <v>-0.95841576099739001</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.94793359488338047</v>
+        <v>-0.94956065635008735</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.9499726910522186</v>
+        <v>-0.94867098943108819</v>
       </c>
       <c r="M3" s="1">
         <v>-0.96</v>
@@ -1106,35 +1106,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.9606429891319348</v>
+        <v>-0.95972948511451028</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96081895131373407</v>
+        <v>-0.95847791013165606</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.9602167930602814</v>
+        <v>-0.96233954119941767</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95921896764939896</v>
+        <v>-0.95872806692106882</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96157758151117811</v>
+        <v>-0.9586593172444301</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96219980961797347</v>
+        <v>-0.95904010264610262</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.95099149126231641</v>
+        <v>-0.94770418425713454</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.95139650258649611</v>
+        <v>-0.95189494573142852</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1146,35 +1146,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.9624852757267075</v>
+        <v>-0.95805368399334789</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95777282583107903</v>
+        <v>-0.95891170965450889</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.9583104592202859</v>
+        <v>-0.96230691410302094</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.9597921611735829</v>
+        <v>-0.95775693553102859</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95867228074841004</v>
+        <v>-0.96056183617094315</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95847198762829711</v>
+        <v>-0.95919688667620939</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.94773297904294174</v>
+        <v>-0.95087101455296186</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.95177379103783621</v>
+        <v>-0.94784402345261143</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1184,35 +1184,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95805757363412614</v>
+        <v>-0.95921305366279819</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96193430372329225</v>
+        <v>-0.96138018864399044</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95867316462497609</v>
+        <v>-0.95969204030875743</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.95993917752131608</v>
+        <v>-0.96203588505242055</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96127376481399329</v>
+        <v>-0.9602512063874028</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.96150745337300236</v>
+        <v>-0.95878563195795874</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.94964681176721888</v>
+        <v>-0.94842487911339135</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-0.94780258950210339</v>
+        <v>-0.95104587942581831</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1312,35 +1312,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4485196993246081</v>
+        <v>3.4380256356657775</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4499738516776692</v>
+        <v>3.4351530437058346</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4387604595007804</v>
+        <v>3.4779856775631717</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4668995229085464</v>
+        <v>3.481817513374077</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4706778105528198</v>
+        <v>3.4658502973660048</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4669126041752341</v>
+        <v>3.4767822991794244</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0513867130596966</v>
+        <v>3.0051015200870506</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0444186757522722</v>
+        <v>3.0487548174657322</v>
       </c>
       <c r="M3">
         <v>3.46</v>
@@ -1356,35 +1356,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.458460023896647</v>
+        <v>3.4774856542884569</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4477544939489335</v>
+        <v>3.4383932203318905</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4554533457252776</v>
+        <v>3.4768626077626013</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4470197669399618</v>
+        <v>3.4736413636262364</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4472954209458613</v>
+        <v>3.4352443231437362</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4370479913458754</v>
+        <v>3.4458280802509047</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0214119258460559</v>
+        <v>3.0409798636803735</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0329637873469464</v>
+        <v>3.0234908218575041</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1396,35 +1396,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4646168117423195</v>
+        <v>3.4451907384125828</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4641019349534261</v>
+        <v>3.4828140420684353</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4494479813452115</v>
+        <v>3.4544601241769719</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4778494385838865</v>
+        <v>3.4439384434611489</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4780141533248519</v>
+        <v>3.4529424481676081</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4408001470945835</v>
+        <v>3.4520755582905425</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0187666194659499</v>
+        <v>3.0262285739542603</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0474523794823476</v>
+        <v>3.0168405061097929</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1434,35 +1434,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4658566740506838</v>
+        <v>3.4402012339812127</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4803999563715613</v>
+        <v>3.4714173713140912</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4441567863160105</v>
+        <v>3.445537349053132</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4366208702041048</v>
+        <v>3.4792787002418097</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4378709969064976</v>
+        <v>3.4515967994518557</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>3.4791771061481866</v>
+        <v>3.4471446208112431</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0201280530665833</v>
+        <v>3.0128722104865657</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>3.0113204740961597</v>
+        <v>3.0475414875979818</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1562,35 +1562,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63147226027360082</v>
+        <v>0.63326914645279364</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63758171014109866</v>
+        <v>0.63687067373689077</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63118052137220337</v>
+        <v>0.6375692835413076</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6331007882880304</v>
+        <v>0.6363311215614591</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63224059348342065</v>
+        <v>0.63289897335272172</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63821167430428538</v>
+        <v>0.63976096164486096</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73505525490275325</v>
+        <v>0.73501666124240961</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73674146120038986</v>
+        <v>0.73662298683288874</v>
       </c>
       <c r="M3">
         <v>0.63500000000000001</v>
@@ -1606,35 +1606,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63335855532160712</v>
+        <v>0.63626648693033105</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63523030747208087</v>
+        <v>0.63174516293985961</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63342355029310915</v>
+        <v>0.63426556287216285</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63484071155943822</v>
+        <v>0.6384168864275982</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63260022667769544</v>
+        <v>0.63078564961511396</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63041460305536046</v>
+        <v>0.63621267947737026</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.72760074988904888</v>
+        <v>0.72936234942990164</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.729999118971706</v>
+        <v>0.734715054109361</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1646,35 +1646,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63456529647437754</v>
+        <v>0.63621589925369404</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63802022708129469</v>
+        <v>0.63791777029789232</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63120188888729822</v>
+        <v>0.63167790699900772</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63570674806614591</v>
+        <v>0.63875448839957794</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63568016215579948</v>
+        <v>0.63585086684724867</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63027281262996404</v>
+        <v>0.63758882192319577</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73210164915804421</v>
+        <v>0.73125045915179732</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73295947537701911</v>
+        <v>0.73364535134943665</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1684,35 +1684,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63756127188282985</v>
+        <v>0.63119273195432757</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63542832881550071</v>
+        <v>0.63246387223567591</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.6312518495385453</v>
+        <v>0.63950894651726564</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63628669609603072</v>
+        <v>0.63338716939652451</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63022492253143891</v>
+        <v>0.63753536768539676</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>0.63239049127496882</v>
+        <v>0.63439798141934278</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73623609220641506</v>
+        <v>0.73245526308925024</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>0.73535814623765605</v>
+        <v>0.73156325287545987</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1812,35 +1812,35 @@
       </c>
       <c r="C3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99579531924733466</v>
+        <v>-0.99698870116153504</v>
       </c>
       <c r="D3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99606937178508959</v>
+        <v>-0.99630881042784858</v>
       </c>
       <c r="E3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99560341509862971</v>
+        <v>-0.9953908695768533</v>
       </c>
       <c r="F3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99646143408267918</v>
+        <v>-0.99685339184400723</v>
       </c>
       <c r="G3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99599446457592911</v>
+        <v>-0.995081813869789</v>
       </c>
       <c r="H3" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99639688633480328</v>
+        <v>-0.99645995996072456</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0294387602370161</v>
+        <v>-1.0304684385741993</v>
       </c>
       <c r="J3" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0300184182859304</v>
+        <v>-1.0302265840061546</v>
       </c>
       <c r="M3">
         <v>-0.996</v>
@@ -1856,35 +1856,35 @@
       </c>
       <c r="C4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99541793441233151</v>
+        <v>-0.99641861685924615</v>
       </c>
       <c r="D4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99505034210158272</v>
+        <v>-0.99662296921023741</v>
       </c>
       <c r="E4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99511412956740952</v>
+        <v>-0.99625443685416992</v>
       </c>
       <c r="F4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99606681082754311</v>
+        <v>-0.99665288957892995</v>
       </c>
       <c r="G4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99680420998928188</v>
+        <v>-0.99693795174766997</v>
       </c>
       <c r="H4" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99687349848929274</v>
+        <v>-0.99641317871086432</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0308023417490613</v>
+        <v>-1.0290706528864726</v>
       </c>
       <c r="J4" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0304339319415114</v>
+        <v>-1.029245223578739</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1896,35 +1896,35 @@
       </c>
       <c r="C5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99580722917773179</v>
+        <v>-0.99578151022968664</v>
       </c>
       <c r="D5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99629006685799582</v>
+        <v>-0.9965817701828078</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.9955716574283483</v>
+        <v>-0.99586492198796539</v>
       </c>
       <c r="F5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99680659665325344</v>
+        <v>-0.99556994652015141</v>
       </c>
       <c r="G5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99664620958676531</v>
+        <v>-0.99660631177678172</v>
       </c>
       <c r="H5" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99514495104538647</v>
+        <v>-0.99529422941259771</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0295241639764319</v>
+        <v>-1.0302213351625824</v>
       </c>
       <c r="J5" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0305407984594483</v>
+        <v>-1.0294380097269489</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1934,35 +1934,35 @@
       </c>
       <c r="C6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99558649562670409</v>
+        <v>-0.99660777671958578</v>
       </c>
       <c r="D6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99692119982833949</v>
+        <v>-0.9960297606762023</v>
       </c>
       <c r="E6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99583110370696681</v>
+        <v>-0.99686386485659795</v>
       </c>
       <c r="F6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99659734772119157</v>
+        <v>-0.99544970881649497</v>
       </c>
       <c r="G6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99658291917533948</v>
+        <v>-0.99609561769236932</v>
       </c>
       <c r="H6" s="4">
         <f ca="1">RAND()*L2 + M2</f>
-        <v>-0.99620965779209958</v>
+        <v>-0.99601245859096033</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0291624416105256</v>
+        <v>-1.0292162212445743</v>
       </c>
       <c r="J6" s="5">
         <f ca="1">RAND()*L2 + N2</f>
-        <v>-1.0290838190656681</v>
+        <v>-1.0297674902914495</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1978,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFA83F3-0FBD-0D45-97C4-EF8BEFA421EA}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1997,101 +1997,201 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <f ca="1">35.6+0.4*RAND()</f>
-        <v>35.757968808335768</v>
+        <v>35.694327540891891</v>
       </c>
       <c r="B2">
         <f ca="1">51.7+RAND()</f>
-        <v>52.668701343682606</v>
+        <v>52.184646554439951</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f t="shared" ref="A3:A11" ca="1" si="0">35.6+0.4*RAND()</f>
-        <v>35.842868588525299</v>
+        <f t="shared" ref="A3:A21" ca="1" si="0">35.6+0.4*RAND()</f>
+        <v>35.940535394996814</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B11" ca="1" si="1">51.7+RAND()</f>
-        <v>52.414718272066246</v>
+        <f t="shared" ref="B3:B21" ca="1" si="1">51.7+RAND()</f>
+        <v>52.524404914518954</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>35.655982749290658</v>
+        <v>35.927970740508478</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>52.261360643278458</v>
+        <v>52.35226242035003</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>35.761600390202517</v>
+        <v>35.88963820272285</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>52.398145527538524</v>
+        <v>52.377668549347668</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>35.696888124635841</v>
+        <v>35.661977525780294</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>52.2424300664361</v>
+        <v>52.494805909752039</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>35.704621614207412</v>
+        <v>35.843786042995447</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>52.341823640499115</v>
+        <v>52.273623246673466</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>35.934076368199165</v>
+        <v>35.75676235722235</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>51.724055459198773</v>
+        <v>52.41487337737756</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>35.83103961027313</v>
+        <v>35.847444499572426</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>51.976528408571554</v>
+        <v>52.247484405077302</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>35.625354702368085</v>
+        <v>35.982047953989444</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>52.179657000466605</v>
+        <v>52.276980855054894</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>35.965566291946935</v>
+        <v>35.986760255499775</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>52.185861466658764</v>
+        <v>51.92910609100695</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" ca="1" si="0"/>
+        <v>35.833565702013686</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ca="1" si="1"/>
+        <v>52.277553753864574</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" ca="1" si="0"/>
+        <v>35.931851457215465</v>
+      </c>
+      <c r="B13">
+        <f t="shared" ca="1" si="1"/>
+        <v>51.768062371327005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" ca="1" si="0"/>
+        <v>35.916675063911072</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ca="1" si="1"/>
+        <v>52.289138594874295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" ca="1" si="0"/>
+        <v>35.769938198973414</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ca="1" si="1"/>
+        <v>52.25427897747835</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" ca="1" si="0"/>
+        <v>35.71595720700482</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ca="1" si="1"/>
+        <v>52.507324947177693</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" ca="1" si="0"/>
+        <v>35.991040897176809</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ca="1" si="1"/>
+        <v>52.194784454041262</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" ca="1" si="0"/>
+        <v>35.935530819021245</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ca="1" si="1"/>
+        <v>52.258805768888038</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" ca="1" si="0"/>
+        <v>35.831326244662719</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ca="1" si="1"/>
+        <v>51.732004611840864</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" ca="1" si="0"/>
+        <v>35.925984094451984</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ca="1" si="1"/>
+        <v>52.136178174181303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" ca="1" si="0"/>
+        <v>35.901205471370673</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ca="1" si="1"/>
+        <v>51.867091823770998</v>
       </c>
     </row>
   </sheetData>
@@ -2103,7 +2203,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32E20358-110C-584C-AD76-D34B5149820A}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>